<commit_message>
impureza de gini adicionada
</commit_message>
<xml_diff>
--- a/arvore_decisao.xlsx
+++ b/arvore_decisao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayumi\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB69D22-2EAC-4003-9680-A57EA8075B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AA1558-73F3-4817-B698-9098E0AB2286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FCFC44A9-22EF-4FFE-A4AF-2B4301E93609}"/>
   </bookViews>
@@ -26,15 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
   <si>
     <t>caro?</t>
   </si>
   <si>
     <t>sim|não</t>
-  </si>
-  <si>
-    <t>57|76</t>
   </si>
   <si>
     <t>quartos&lt;=3?</t>
@@ -43,40 +40,31 @@
     <t>banheiros&gt;=2.5?</t>
   </si>
   <si>
-    <t>16|24</t>
-  </si>
-  <si>
-    <t>74|87</t>
-  </si>
-  <si>
-    <t>54|66</t>
-  </si>
-  <si>
     <t>sqft_living&lt;=1435?</t>
-  </si>
-  <si>
-    <t>36|45</t>
-  </si>
-  <si>
-    <t>33|35</t>
-  </si>
-  <si>
-    <t>13|8</t>
   </si>
   <si>
     <t>sqft_lot&lt;=11000?</t>
   </si>
   <si>
-    <t>77|103</t>
-  </si>
-  <si>
     <t>floors&lt;2?</t>
   </si>
   <si>
-    <t>67|76</t>
+    <t>views==2?</t>
   </si>
   <si>
-    <t>23|35</t>
+    <t>condition&gt;3?</t>
+  </si>
+  <si>
+    <t>grade&gt;4?</t>
+  </si>
+  <si>
+    <t>impureza de gini</t>
+  </si>
+  <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>não</t>
   </si>
 </sst>
 </file>
@@ -192,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -201,16 +189,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5093,192 +5083,565 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF305A8-9ACD-425D-8321-92328A7792B8}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9" t="s">
-        <v>11</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5">
+        <v>76</v>
+      </c>
+      <c r="C4" s="9">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <f>1-((A4/(B4+A4))^2)-((B4/(A4+B4))^2)</f>
+        <v>0.48979591836734698</v>
+      </c>
+      <c r="H4">
+        <f>1-((C4/(D4+C4))^2)-((D4/(C4+D4))^2)</f>
+        <v>0.49956747404844298</v>
+      </c>
+      <c r="J4">
+        <f>((A4+B4)/199)*F4+((C4+D4)/199)*H4</f>
+        <v>0.49805751446307167</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7">
+        <v>35</v>
+      </c>
+      <c r="C8" s="10">
+        <v>67</v>
+      </c>
+      <c r="D8" s="11">
+        <v>76</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F5:F36" si="0">1-((A8/(B8+A8))^2)-((B8/(A8+B8))^2)</f>
+        <v>0.47859690844233055</v>
+      </c>
+      <c r="H8">
+        <f>1-((C8/(D8+C8))^2)-((D8/(C8+D8))^2)</f>
+        <v>0.49801946305442812</v>
+      </c>
+      <c r="J8">
+        <f>((A8+B8)/199)*F8+((C8+D8)/199)*H8</f>
+        <v>0.49736383872582107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D10" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>36</v>
+      </c>
+      <c r="B12" s="7">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10">
+        <v>54</v>
+      </c>
+      <c r="D12" s="11">
+        <v>84</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.48979591836734704</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12" si="1">1-((C12/(D12+C12))^2)-((D12/(C12+D12))^2)</f>
+        <v>0.47637051039697537</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J5:J36" si="2">((A12+B12)/199)*F12+((C12+D12)/199)*H12</f>
+        <v>0.48540840850213801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7">
+        <v>30</v>
+      </c>
+      <c r="C16" s="10">
+        <v>16</v>
+      </c>
+      <c r="D16" s="11">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.47480216576426493</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16" si="3">1-((C16/(D16+C16))^2)-((D16/(C16+D16))^2)</f>
+        <v>0.48</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0.21339349810275871</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="D19" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
-        <v>15</v>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7">
+        <v>35</v>
+      </c>
+      <c r="C20" s="10">
+        <v>67</v>
+      </c>
+      <c r="D20" s="11">
+        <v>76</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.47859690844233055</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20" si="4">1-((C20/(D20+C20))^2)-((D20/(C20+D20))^2)</f>
+        <v>0.49801946305442812</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0.49736383872582107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>36</v>
+      </c>
+      <c r="B24" s="7">
+        <v>45</v>
+      </c>
+      <c r="C24" s="10">
+        <v>54</v>
+      </c>
+      <c r="D24" s="11">
+        <v>66</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.49382716049382713</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24" si="5">1-((C24/(D24+C24))^2)-((D24/(C24+D24))^2)</f>
+        <v>0.49499999999999994</v>
+      </c>
+      <c r="J24">
+        <f>((A24+B24)/199)*F24+((C24+D24)/199)*H24</f>
+        <v>0.49949748743718586</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10">
+        <v>89</v>
+      </c>
+      <c r="D28" s="11">
+        <v>110</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ref="H28" si="6">1-((C28/(D28+C28))^2)-((D28/(C28+D28))^2)</f>
+        <v>0.49443195878891955</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>0.49443195878891955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>77</v>
+      </c>
+      <c r="B32" s="7">
+        <v>103</v>
+      </c>
+      <c r="C32" s="10">
+        <v>13</v>
+      </c>
+      <c r="D32" s="11">
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0.48956790123456795</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ref="H32" si="7">1-((C32/(D32+C32))^2)-((D32/(C32+D32))^2)</f>
+        <v>0.47165532879818595</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>0.49259791018584992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>64</v>
+      </c>
+      <c r="B36" s="7">
+        <v>62</v>
+      </c>
+      <c r="C36" s="10">
+        <v>26</v>
+      </c>
+      <c r="D36" s="11">
+        <v>49</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0.49987402368354755</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36" si="8">1-((C36/(D36+C36))^2)-((D36/(C36+D36))^2)</f>
+        <v>0.45297777777777776</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>0.48722341868070518</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>64</v>
+      </c>
+      <c r="B40" s="7">
+        <v>62</v>
+      </c>
+      <c r="C40" s="10">
+        <v>26</v>
+      </c>
+      <c r="D40" s="11">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>